<commit_message>
Add: Total BOM price sum
</commit_message>
<xml_diff>
--- a/Schematics/BOM_IoT.xlsx
+++ b/Schematics/BOM_IoT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Documents\ITESO\10Semestre\IoT\git\Schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16705476-DDBE-4A5B-BAE3-C031B8746BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554B418A-4C78-4857-9E40-F2358C6AE5FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="301">
   <si>
     <t>NA</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>U.FL-R-SMT-1(60)</t>
-  </si>
-  <si>
-    <t>UFL</t>
   </si>
   <si>
     <t>L1</t>
@@ -940,6 +937,9 @@
   <si>
     <t>https://www.digikey.com/products/en?mpart=328&amp;v=1528</t>
   </si>
+  <si>
+    <t>Total price:</t>
+  </si>
 </sst>
 </file>
 
@@ -1051,7 +1051,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1233,13 +1233,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1272,7 +1315,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1341,6 +1383,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1633,8 +1678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW695"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1673,44 +1718,44 @@
     </row>
     <row r="2" spans="1:49" ht="13.5" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="64" t="s">
+      <c r="G2" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="H2" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="64" t="s">
+      <c r="J2" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="64" t="s">
+      <c r="K2" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="64" t="s">
-        <v>183</v>
-      </c>
-      <c r="M2" s="65" t="s">
+      <c r="L2" s="63" t="s">
+        <v>182</v>
+      </c>
+      <c r="M2" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="66" t="s">
-        <v>83</v>
+      <c r="N2" s="65" t="s">
+        <v>82</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -1750,42 +1795,42 @@
     </row>
     <row r="3" spans="1:49" ht="30">
       <c r="A3" s="1"/>
-      <c r="B3" s="21">
+      <c r="B3" s="20">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <v>1</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <v>0.63400000000000001</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="22">
         <f>D3*E3</f>
         <v>0.63400000000000001</v>
       </c>
-      <c r="G3" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" s="22" t="s">
+      <c r="G3" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="L3" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="M3" s="23" t="s">
         <v>71</v>
-      </c>
-      <c r="M3" s="24" t="s">
-        <v>72</v>
       </c>
       <c r="N3" s="12"/>
       <c r="O3" s="3"/>
@@ -1826,42 +1871,42 @@
     </row>
     <row r="4" spans="1:49" ht="39">
       <c r="A4" s="1"/>
-      <c r="B4" s="25">
+      <c r="B4" s="24">
         <v>2</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="26">
         <v>12</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="27">
         <v>0.156</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="27">
         <f t="shared" ref="F4:F55" si="0">D4*E4</f>
         <v>1.8719999999999999</v>
       </c>
-      <c r="G4" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" s="27" t="s">
+      <c r="G4" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="L4" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="29" t="s">
         <v>77</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M4" s="30" t="s">
-        <v>78</v>
       </c>
       <c r="N4" s="14"/>
       <c r="O4" s="3"/>
@@ -1902,42 +1947,42 @@
     </row>
     <row r="5" spans="1:49" ht="30">
       <c r="A5" s="1"/>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>3</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="26">
         <v>2</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="27">
         <v>0.247</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <f t="shared" si="0"/>
         <v>0.49399999999999999</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="29" t="s">
+      <c r="K5" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="29" t="s">
         <v>81</v>
-      </c>
-      <c r="K5" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="L5" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M5" s="30" t="s">
-        <v>82</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="3"/>
@@ -1978,45 +2023,45 @@
     </row>
     <row r="6" spans="1:49" ht="30">
       <c r="A6" s="1"/>
-      <c r="B6" s="25">
+      <c r="B6" s="24">
         <v>4</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <v>2</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="27">
         <v>0.13</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="27">
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="K6" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="L6" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M6" s="30" t="s">
+      <c r="N6" s="14" t="s">
         <v>86</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>87</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -2056,45 +2101,45 @@
     </row>
     <row r="7" spans="1:49" ht="30">
       <c r="A7" s="1"/>
-      <c r="B7" s="25">
+      <c r="B7" s="24">
         <v>5</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="26">
         <v>1</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="27">
         <v>0.13</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="27">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="27" t="s">
+      <c r="K7" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="L7" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M7" s="30" t="s">
-        <v>91</v>
-      </c>
       <c r="N7" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -2134,42 +2179,42 @@
     </row>
     <row r="8" spans="1:49" ht="45">
       <c r="A8" s="1"/>
-      <c r="B8" s="25">
+      <c r="B8" s="24">
         <v>6</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="26">
         <v>4</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="27">
         <v>0.56000000000000005</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="27">
         <f t="shared" si="0"/>
         <v>2.2400000000000002</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="27" t="s">
+      <c r="K8" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8" s="29" t="s">
         <v>94</v>
-      </c>
-      <c r="K8" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="L8" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M8" s="30" t="s">
-        <v>95</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="3"/>
@@ -2210,42 +2255,42 @@
     </row>
     <row r="9" spans="1:49" ht="45">
       <c r="A9" s="1"/>
-      <c r="B9" s="25">
+      <c r="B9" s="24">
         <v>7</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="26">
         <v>4</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="27">
         <v>0.13</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="27">
         <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M9" s="29" t="s">
         <v>97</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="K9" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="L9" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M9" s="30" t="s">
-        <v>98</v>
       </c>
       <c r="N9" s="14"/>
       <c r="O9" s="3"/>
@@ -2286,42 +2331,42 @@
     </row>
     <row r="10" spans="1:49" ht="30">
       <c r="A10" s="1"/>
-      <c r="B10" s="25">
+      <c r="B10" s="24">
         <v>8</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="26">
         <v>1</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <v>0.13</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="27">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M10" s="29" t="s">
         <v>100</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="K10" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="L10" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M10" s="30" t="s">
-        <v>101</v>
       </c>
       <c r="N10" s="14"/>
       <c r="O10" s="3"/>
@@ -2362,42 +2407,42 @@
     </row>
     <row r="11" spans="1:49" ht="45">
       <c r="A11" s="1"/>
-      <c r="B11" s="25">
+      <c r="B11" s="24">
         <v>9</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="26">
         <v>1</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="27">
         <v>0.2</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="27">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="L11" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M11" s="29" t="s">
         <v>103</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="K11" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M11" s="30" t="s">
-        <v>104</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="3"/>
@@ -2438,42 +2483,42 @@
     </row>
     <row r="12" spans="1:49" ht="45">
       <c r="A12" s="1"/>
-      <c r="B12" s="25">
+      <c r="B12" s="24">
         <v>10</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="26">
         <v>1</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="27">
         <v>0.53</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="27">
         <f t="shared" si="0"/>
         <v>0.53</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="H12" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="27" t="s">
+      <c r="K12" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12" s="29" t="s">
         <v>106</v>
-      </c>
-      <c r="K12" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="L12" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M12" s="30" t="s">
-        <v>107</v>
       </c>
       <c r="N12" s="14"/>
       <c r="O12" s="3"/>
@@ -2514,42 +2559,42 @@
     </row>
     <row r="13" spans="1:49" ht="30">
       <c r="A13" s="1"/>
-      <c r="B13" s="25">
+      <c r="B13" s="24">
         <v>11</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="26">
         <v>1</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="27">
         <v>0.13</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="27">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="H13" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="27" t="s">
+      <c r="K13" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="L13" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M13" s="29" t="s">
         <v>109</v>
-      </c>
-      <c r="K13" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="L13" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M13" s="30" t="s">
-        <v>110</v>
       </c>
       <c r="N13" s="14"/>
       <c r="O13" s="3"/>
@@ -2590,42 +2635,42 @@
     </row>
     <row r="14" spans="1:49" ht="30">
       <c r="A14" s="1"/>
-      <c r="B14" s="25">
+      <c r="B14" s="24">
         <v>12</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="26">
         <v>3</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="27">
         <v>0.99</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="27">
         <f t="shared" si="0"/>
         <v>2.9699999999999998</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="H14" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J14" s="27" t="s">
+      <c r="K14" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="L14" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" s="29" t="s">
         <v>112</v>
-      </c>
-      <c r="K14" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="L14" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M14" s="30" t="s">
-        <v>113</v>
       </c>
       <c r="N14" s="14"/>
       <c r="O14" s="3"/>
@@ -2666,42 +2711,42 @@
     </row>
     <row r="15" spans="1:49" ht="45">
       <c r="A15" s="1"/>
-      <c r="B15" s="25">
+      <c r="B15" s="24">
         <v>13</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="26">
         <v>1</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="27">
         <v>0.13</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="27">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M15" s="29" t="s">
         <v>115</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="K15" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="L15" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M15" s="30" t="s">
-        <v>116</v>
       </c>
       <c r="N15" s="14"/>
       <c r="O15" s="3"/>
@@ -2742,42 +2787,42 @@
     </row>
     <row r="16" spans="1:49" ht="30">
       <c r="A16" s="1"/>
-      <c r="B16" s="31">
+      <c r="B16" s="30">
         <v>14</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="31">
         <v>1</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="32">
         <v>0.66</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="32">
         <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
-      <c r="G16" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="H16" s="32" t="s">
+      <c r="G16" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="H16" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="32" t="s">
+      <c r="I16" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="32" t="s">
+      <c r="J16" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="K16" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="K16" s="32" t="s">
+      <c r="L16" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="M16" s="33" t="s">
         <v>118</v>
-      </c>
-      <c r="L16" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="M16" s="34" t="s">
-        <v>119</v>
       </c>
       <c r="N16" s="14"/>
       <c r="O16" s="3"/>
@@ -2818,42 +2863,42 @@
     </row>
     <row r="17" spans="1:49" ht="30">
       <c r="A17" s="1"/>
-      <c r="B17" s="31">
+      <c r="B17" s="30">
         <v>15</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="31">
         <v>2</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="32">
         <v>0.59</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="32">
         <f t="shared" si="0"/>
         <v>1.18</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="H17" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="I17" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="J17" s="32" t="s">
+      <c r="K17" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="L17" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="M17" s="33" t="s">
         <v>122</v>
-      </c>
-      <c r="K17" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="L17" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="M17" s="34" t="s">
-        <v>123</v>
       </c>
       <c r="N17" s="14"/>
       <c r="O17" s="3"/>
@@ -2894,42 +2939,42 @@
     </row>
     <row r="18" spans="1:49" ht="30">
       <c r="A18" s="1"/>
-      <c r="B18" s="31">
+      <c r="B18" s="30">
         <v>16</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="31">
         <v>3</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="32">
         <v>0.66</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="32">
         <f t="shared" si="0"/>
         <v>1.98</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="H18" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="32" t="s">
+      <c r="K18" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="K18" s="32" t="s">
+      <c r="L18" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="M18" s="33" t="s">
         <v>126</v>
-      </c>
-      <c r="L18" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="M18" s="34" t="s">
-        <v>127</v>
       </c>
       <c r="N18" s="14"/>
       <c r="O18" s="3"/>
@@ -2969,42 +3014,42 @@
       <c r="AW18" s="3"/>
     </row>
     <row r="19" spans="1:49" ht="30">
-      <c r="B19" s="31">
+      <c r="B19" s="30">
         <v>17</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="31">
         <v>1</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="32">
         <v>0.53</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="32">
         <f t="shared" si="0"/>
         <v>0.53</v>
       </c>
-      <c r="G19" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="H19" s="32" t="s">
+      <c r="G19" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="32" t="s">
+      <c r="I19" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J19" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="K19" s="32" t="s">
+      <c r="J19" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="K19" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="L19" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="M19" s="33" t="s">
         <v>132</v>
-      </c>
-      <c r="L19" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="M19" s="34" t="s">
-        <v>133</v>
       </c>
       <c r="N19" s="14"/>
       <c r="O19" s="3"/>
@@ -3044,42 +3089,42 @@
       <c r="AW19" s="3"/>
     </row>
     <row r="20" spans="1:49" ht="30">
-      <c r="B20" s="31">
+      <c r="B20" s="30">
         <v>18</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="31">
         <v>1</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="32">
         <v>0.53</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="32">
         <f t="shared" si="0"/>
         <v>0.53</v>
       </c>
-      <c r="G20" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="H20" s="32" t="s">
+      <c r="G20" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="32" t="s">
+      <c r="I20" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J20" s="35" t="s">
+      <c r="J20" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="K20" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="L20" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="M20" s="33" t="s">
         <v>134</v>
-      </c>
-      <c r="K20" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="L20" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="M20" s="34" t="s">
-        <v>135</v>
       </c>
       <c r="N20" s="14"/>
       <c r="O20" s="3"/>
@@ -3119,42 +3164,42 @@
       <c r="AW20" s="3"/>
     </row>
     <row r="21" spans="1:49" ht="30">
-      <c r="B21" s="31">
+      <c r="B21" s="30">
         <v>19</v>
       </c>
-      <c r="C21" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="D21" s="32">
+      <c r="C21" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="31">
         <v>2</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="32">
         <v>0.53</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="32">
         <f t="shared" si="0"/>
         <v>1.06</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="K21" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="H21" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="I21" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="J21" s="32" t="s">
+      <c r="L21" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="M21" s="33" t="s">
         <v>136</v>
-      </c>
-      <c r="K21" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="L21" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="M21" s="34" t="s">
-        <v>137</v>
       </c>
       <c r="N21" s="14"/>
       <c r="O21" s="3"/>
@@ -3194,42 +3239,42 @@
       <c r="AW21" s="3"/>
     </row>
     <row r="22" spans="1:49" ht="30">
-      <c r="B22" s="31">
+      <c r="B22" s="30">
         <v>20</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="31">
         <v>1</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="32">
         <v>0.82</v>
       </c>
-      <c r="F22" s="33">
+      <c r="F22" s="32">
         <f t="shared" si="0"/>
         <v>0.82</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="I22" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="K22" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="L22" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="M22" s="33" t="s">
         <v>140</v>
-      </c>
-      <c r="H22" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="I22" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="J22" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="K22" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="L22" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="M22" s="34" t="s">
-        <v>141</v>
       </c>
       <c r="N22" s="14"/>
       <c r="O22" s="3"/>
@@ -3269,42 +3314,42 @@
       <c r="AW22" s="3"/>
     </row>
     <row r="23" spans="1:49" ht="30">
-      <c r="B23" s="36">
+      <c r="B23" s="35">
         <v>21</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="37">
+      <c r="D23" s="36">
         <v>1</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="37">
         <v>1.04</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="37">
         <f t="shared" si="0"/>
         <v>1.04</v>
       </c>
-      <c r="G23" s="37" t="s">
+      <c r="G23" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="H23" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="J23" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="L23" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="M23" s="38" t="s">
         <v>142</v>
-      </c>
-      <c r="H23" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="I23" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="J23" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="K23" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="L23" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="M23" s="39" t="s">
-        <v>143</v>
       </c>
       <c r="N23" s="14"/>
       <c r="O23" s="3"/>
@@ -3344,42 +3389,42 @@
       <c r="AW23" s="3"/>
     </row>
     <row r="24" spans="1:49" ht="30">
-      <c r="B24" s="36">
+      <c r="B24" s="35">
         <v>22</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="37">
+      <c r="D24" s="36">
         <v>1</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="37">
         <v>1.43</v>
       </c>
-      <c r="F24" s="38">
+      <c r="F24" s="37">
         <f t="shared" si="0"/>
         <v>1.43</v>
       </c>
-      <c r="G24" s="37" t="s">
+      <c r="G24" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="H24" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="J24" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="K24" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="L24" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="M24" s="38" t="s">
         <v>144</v>
-      </c>
-      <c r="H24" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="I24" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="J24" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="K24" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="L24" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="M24" s="39" t="s">
-        <v>145</v>
       </c>
       <c r="N24" s="14"/>
       <c r="O24" s="3"/>
@@ -3419,42 +3464,42 @@
       <c r="AW24" s="3"/>
     </row>
     <row r="25" spans="1:49" ht="30">
-      <c r="B25" s="36">
+      <c r="B25" s="35">
         <v>23</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="37">
+      <c r="D25" s="36">
         <v>1</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="37">
         <v>0.57999999999999996</v>
       </c>
-      <c r="F25" s="38">
+      <c r="F25" s="37">
         <f t="shared" si="0"/>
         <v>0.57999999999999996</v>
       </c>
-      <c r="G25" s="37" t="s">
+      <c r="G25" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="H25" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="J25" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="K25" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="H25" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="I25" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="J25" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="K25" s="37" t="s">
+      <c r="L25" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="L25" s="37" t="s">
+      <c r="M25" s="38" t="s">
         <v>149</v>
-      </c>
-      <c r="M25" s="39" t="s">
-        <v>150</v>
       </c>
       <c r="N25" s="14"/>
       <c r="O25" s="3"/>
@@ -3494,42 +3539,42 @@
       <c r="AW25" s="3"/>
     </row>
     <row r="26" spans="1:49" ht="45">
-      <c r="B26" s="40">
+      <c r="B26" s="39">
         <v>24</v>
       </c>
-      <c r="C26" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="41">
+      <c r="C26" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="40">
         <v>1</v>
       </c>
-      <c r="E26" s="42">
+      <c r="E26" s="41">
         <v>0.13</v>
       </c>
-      <c r="F26" s="42">
+      <c r="F26" s="41">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="G26" s="41" t="s">
+      <c r="G26" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="H26" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="I26" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="K26" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="L26" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="M26" s="42" t="s">
         <v>151</v>
-      </c>
-      <c r="H26" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="I26" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="K26" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="L26" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="M26" s="43" t="s">
-        <v>152</v>
       </c>
       <c r="N26" s="14"/>
       <c r="O26" s="3"/>
@@ -3569,42 +3614,42 @@
       <c r="AW26" s="3"/>
     </row>
     <row r="27" spans="1:49" ht="30">
-      <c r="B27" s="40">
+      <c r="B27" s="39">
         <v>25</v>
       </c>
-      <c r="C27" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="41">
+      <c r="C27" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="40">
         <v>1</v>
       </c>
-      <c r="E27" s="42">
+      <c r="E27" s="41">
         <v>0.7</v>
       </c>
-      <c r="F27" s="42">
+      <c r="F27" s="41">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="G27" s="41" t="s">
+      <c r="G27" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="H27" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="J27" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="K27" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="H27" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="I27" s="44" t="s">
-        <v>158</v>
-      </c>
-      <c r="J27" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="K27" s="41" t="s">
+      <c r="L27" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="M27" s="42" t="s">
         <v>155</v>
-      </c>
-      <c r="L27" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="M27" s="43" t="s">
-        <v>156</v>
       </c>
       <c r="N27" s="14"/>
       <c r="O27" s="3"/>
@@ -3644,42 +3689,42 @@
       <c r="AW27" s="3"/>
     </row>
     <row r="28" spans="1:49" ht="45">
-      <c r="B28" s="40">
+      <c r="B28" s="39">
         <v>26</v>
       </c>
-      <c r="C28" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="41">
+      <c r="C28" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="40">
         <v>2</v>
       </c>
-      <c r="E28" s="42">
+      <c r="E28" s="41">
         <v>0.13</v>
       </c>
-      <c r="F28" s="42">
+      <c r="F28" s="41">
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="G28" s="41" t="s">
+      <c r="G28" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="H28" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="H28" s="41" t="s">
+      <c r="I28" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="K28" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="L28" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="M28" s="42" t="s">
         <v>161</v>
-      </c>
-      <c r="I28" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="J28" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="K28" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="L28" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="M28" s="43" t="s">
-        <v>162</v>
       </c>
       <c r="N28" s="14"/>
       <c r="O28" s="3"/>
@@ -3719,42 +3764,42 @@
       <c r="AW28" s="3"/>
     </row>
     <row r="29" spans="1:49" ht="30">
-      <c r="B29" s="31">
+      <c r="B29" s="30">
         <v>27</v>
       </c>
-      <c r="C29" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="D29" s="32">
+      <c r="C29" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="31">
         <v>1</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="32">
         <v>1</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G29" s="32" t="s">
+      <c r="G29" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="H29" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="I29" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="K29" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="L29" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="M29" s="33" t="s">
         <v>169</v>
-      </c>
-      <c r="I29" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="J29" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="K29" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="L29" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="M29" s="34" t="s">
-        <v>170</v>
       </c>
       <c r="N29" s="14"/>
       <c r="O29" s="3"/>
@@ -3798,7 +3843,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D30" s="5">
         <v>1</v>
@@ -3811,7 +3856,7 @@
         <v>0.6</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>0</v>
@@ -3820,16 +3865,16 @@
         <v>59</v>
       </c>
       <c r="J30" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="K30" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M30" s="10" t="s">
         <v>166</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="M30" s="10" t="s">
-        <v>167</v>
       </c>
       <c r="N30" s="14"/>
       <c r="O30" s="3"/>
@@ -3869,42 +3914,42 @@
       <c r="AW30" s="3"/>
     </row>
     <row r="31" spans="1:49" ht="30">
-      <c r="B31" s="47">
+      <c r="B31" s="46">
         <v>29</v>
       </c>
-      <c r="C31" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="D31" s="48">
+      <c r="C31" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="47">
         <v>2</v>
       </c>
-      <c r="E31" s="49">
+      <c r="E31" s="48">
         <v>0.52</v>
       </c>
-      <c r="F31" s="49">
+      <c r="F31" s="48">
         <f t="shared" si="0"/>
         <v>1.04</v>
       </c>
-      <c r="G31" s="48" t="s">
+      <c r="G31" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="H31" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31" s="47" t="s">
         <v>173</v>
       </c>
-      <c r="H31" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="I31" s="48" t="s">
+      <c r="J31" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="J31" s="50" t="s">
+      <c r="K31" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="K31" s="48" t="s">
+      <c r="L31" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="M31" s="50" t="s">
         <v>176</v>
-      </c>
-      <c r="L31" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="M31" s="51" t="s">
-        <v>177</v>
       </c>
       <c r="N31" s="14"/>
       <c r="O31" s="3"/>
@@ -3944,42 +3989,42 @@
       <c r="AW31" s="3"/>
     </row>
     <row r="32" spans="1:49" ht="45">
-      <c r="B32" s="47">
+      <c r="B32" s="46">
         <v>30</v>
       </c>
-      <c r="C32" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="D32" s="48">
+      <c r="C32" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="D32" s="47">
         <v>1</v>
       </c>
-      <c r="E32" s="49">
+      <c r="E32" s="48">
         <v>0.65</v>
       </c>
-      <c r="F32" s="49">
+      <c r="F32" s="48">
         <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
-      <c r="G32" s="48" t="s">
+      <c r="G32" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="H32" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="J32" s="47" t="s">
         <v>179</v>
       </c>
-      <c r="H32" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="I32" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="J32" s="48" t="s">
+      <c r="K32" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="K32" s="48" t="s">
+      <c r="L32" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="M32" s="50" t="s">
         <v>181</v>
-      </c>
-      <c r="L32" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="M32" s="51" t="s">
-        <v>182</v>
       </c>
       <c r="N32" s="14"/>
       <c r="O32" s="3"/>
@@ -4019,42 +4064,42 @@
       <c r="AW32" s="3"/>
     </row>
     <row r="33" spans="2:49" ht="30">
-      <c r="B33" s="47">
+      <c r="B33" s="46">
         <v>31</v>
       </c>
-      <c r="C33" s="48" t="s">
-        <v>184</v>
-      </c>
-      <c r="D33" s="48">
+      <c r="C33" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="D33" s="47">
         <v>1</v>
       </c>
-      <c r="E33" s="49">
+      <c r="E33" s="48">
         <v>0.39</v>
       </c>
-      <c r="F33" s="49">
+      <c r="F33" s="48">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
-      <c r="G33" s="48" t="s">
+      <c r="G33" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="H33" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="J33" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="H33" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="I33" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="J33" s="48" t="s">
+      <c r="K33" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="L33" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="M33" s="50" t="s">
         <v>186</v>
-      </c>
-      <c r="K33" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="L33" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="M33" s="51" t="s">
-        <v>187</v>
       </c>
       <c r="N33" s="14"/>
       <c r="O33" s="3"/>
@@ -4094,42 +4139,42 @@
       <c r="AW33" s="3"/>
     </row>
     <row r="34" spans="2:49" ht="15">
-      <c r="B34" s="52">
+      <c r="B34" s="51">
         <v>32</v>
       </c>
-      <c r="C34" s="53" t="s">
-        <v>188</v>
-      </c>
-      <c r="D34" s="53">
+      <c r="C34" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="D34" s="52">
         <v>1</v>
       </c>
-      <c r="E34" s="54">
+      <c r="E34" s="53">
         <v>0.1</v>
       </c>
-      <c r="F34" s="54">
+      <c r="F34" s="53">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G34" s="53" t="s">
+      <c r="G34" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="H34" s="52" t="s">
         <v>189</v>
       </c>
-      <c r="H34" s="53" t="s">
+      <c r="I34" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="55" t="s">
         <v>190</v>
       </c>
-      <c r="I34" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J34" s="56" t="s">
+      <c r="K34" s="52" t="s">
         <v>191</v>
       </c>
-      <c r="K34" s="53" t="s">
+      <c r="L34" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="M34" s="56" t="s">
         <v>192</v>
-      </c>
-      <c r="L34" s="53" t="s">
-        <v>149</v>
-      </c>
-      <c r="M34" s="57" t="s">
-        <v>193</v>
       </c>
       <c r="N34" s="14"/>
       <c r="O34" s="3"/>
@@ -4169,42 +4214,42 @@
       <c r="AW34" s="3"/>
     </row>
     <row r="35" spans="2:49" ht="30">
-      <c r="B35" s="52">
+      <c r="B35" s="51">
         <v>33</v>
       </c>
-      <c r="C35" s="53" t="s">
-        <v>194</v>
-      </c>
-      <c r="D35" s="53">
+      <c r="C35" s="52" t="s">
+        <v>193</v>
+      </c>
+      <c r="D35" s="52">
         <v>3</v>
       </c>
-      <c r="E35" s="54">
+      <c r="E35" s="53">
         <v>0.13</v>
       </c>
-      <c r="F35" s="54">
+      <c r="F35" s="53">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
-      <c r="G35" s="53" t="s">
+      <c r="G35" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="H35" s="52" t="s">
         <v>195</v>
       </c>
-      <c r="H35" s="53" t="s">
+      <c r="I35" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="52" t="s">
         <v>196</v>
       </c>
-      <c r="I35" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J35" s="53" t="s">
+      <c r="K35" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L35" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M35" s="56" t="s">
         <v>197</v>
-      </c>
-      <c r="K35" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="L35" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="M35" s="57" t="s">
-        <v>198</v>
       </c>
       <c r="N35" s="14"/>
       <c r="O35" s="3"/>
@@ -4244,42 +4289,42 @@
       <c r="AW35" s="3"/>
     </row>
     <row r="36" spans="2:49" ht="30">
-      <c r="B36" s="52">
+      <c r="B36" s="51">
         <v>34</v>
       </c>
-      <c r="C36" s="53" t="s">
-        <v>199</v>
-      </c>
-      <c r="D36" s="53">
+      <c r="C36" s="52" t="s">
+        <v>198</v>
+      </c>
+      <c r="D36" s="52">
         <v>3</v>
       </c>
-      <c r="E36" s="54">
+      <c r="E36" s="53">
         <v>0.13</v>
       </c>
-      <c r="F36" s="54">
+      <c r="F36" s="53">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
-      <c r="G36" s="53" t="s">
+      <c r="G36" s="52" t="s">
+        <v>199</v>
+      </c>
+      <c r="H36" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="H36" s="53" t="s">
+      <c r="I36" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="I36" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="53" t="s">
+      <c r="K36" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L36" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M36" s="56" t="s">
         <v>202</v>
-      </c>
-      <c r="K36" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="L36" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="M36" s="57" t="s">
-        <v>203</v>
       </c>
       <c r="N36" s="14"/>
       <c r="O36" s="3"/>
@@ -4319,42 +4364,42 @@
       <c r="AW36" s="3"/>
     </row>
     <row r="37" spans="2:49" ht="30">
-      <c r="B37" s="52">
+      <c r="B37" s="51">
         <v>35</v>
       </c>
-      <c r="C37" s="58" t="s">
-        <v>204</v>
-      </c>
-      <c r="D37" s="53">
+      <c r="C37" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="D37" s="52">
         <v>7</v>
       </c>
-      <c r="E37" s="54">
+      <c r="E37" s="53">
         <v>0.13</v>
       </c>
-      <c r="F37" s="54">
+      <c r="F37" s="53">
         <f t="shared" si="0"/>
         <v>0.91</v>
       </c>
-      <c r="G37" s="53" t="s">
+      <c r="G37" s="52" t="s">
+        <v>204</v>
+      </c>
+      <c r="H37" s="52" t="s">
         <v>205</v>
       </c>
-      <c r="H37" s="53" t="s">
+      <c r="I37" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="52" t="s">
         <v>206</v>
       </c>
-      <c r="I37" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J37" s="53" t="s">
+      <c r="K37" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L37" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M37" s="56" t="s">
         <v>207</v>
-      </c>
-      <c r="K37" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="L37" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="M37" s="57" t="s">
-        <v>208</v>
       </c>
       <c r="N37" s="14"/>
       <c r="O37" s="3"/>
@@ -4394,45 +4439,45 @@
       <c r="AW37" s="3"/>
     </row>
     <row r="38" spans="2:49">
-      <c r="B38" s="52">
+      <c r="B38" s="51">
         <v>36</v>
       </c>
-      <c r="C38" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="D38" s="53">
+      <c r="C38" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="D38" s="52">
         <v>3</v>
       </c>
-      <c r="E38" s="54">
+      <c r="E38" s="53">
         <v>0</v>
       </c>
-      <c r="F38" s="54">
+      <c r="F38" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G38" s="53" t="s">
+      <c r="G38" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="H38" s="52" t="s">
         <v>210</v>
       </c>
-      <c r="H38" s="53" t="s">
+      <c r="I38" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="52" t="s">
+        <v>210</v>
+      </c>
+      <c r="K38" s="52" t="s">
+        <v>210</v>
+      </c>
+      <c r="L38" s="52" t="s">
+        <v>210</v>
+      </c>
+      <c r="M38" s="57" t="s">
+        <v>210</v>
+      </c>
+      <c r="N38" s="14" t="s">
         <v>211</v>
-      </c>
-      <c r="I38" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J38" s="53" t="s">
-        <v>211</v>
-      </c>
-      <c r="K38" s="53" t="s">
-        <v>211</v>
-      </c>
-      <c r="L38" s="53" t="s">
-        <v>211</v>
-      </c>
-      <c r="M38" s="58" t="s">
-        <v>211</v>
-      </c>
-      <c r="N38" s="14" t="s">
-        <v>212</v>
       </c>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
@@ -4471,42 +4516,42 @@
       <c r="AW38" s="3"/>
     </row>
     <row r="39" spans="2:49" ht="30">
-      <c r="B39" s="52">
+      <c r="B39" s="51">
         <v>37</v>
       </c>
-      <c r="C39" s="53" t="s">
-        <v>213</v>
-      </c>
-      <c r="D39" s="53">
+      <c r="C39" s="52" t="s">
+        <v>212</v>
+      </c>
+      <c r="D39" s="52">
         <v>1</v>
       </c>
-      <c r="E39" s="54">
+      <c r="E39" s="53">
         <v>0.13</v>
       </c>
-      <c r="F39" s="54">
+      <c r="F39" s="53">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="G39" s="53" t="s">
+      <c r="G39" s="52" t="s">
+        <v>213</v>
+      </c>
+      <c r="H39" s="52" t="s">
         <v>214</v>
       </c>
-      <c r="H39" s="53" t="s">
+      <c r="I39" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="I39" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="53" t="s">
+      <c r="K39" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L39" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M39" s="56" t="s">
         <v>216</v>
-      </c>
-      <c r="K39" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="L39" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="M39" s="57" t="s">
-        <v>217</v>
       </c>
       <c r="N39" s="14"/>
       <c r="O39" s="3"/>
@@ -4546,42 +4591,42 @@
       <c r="AW39" s="3"/>
     </row>
     <row r="40" spans="2:49" ht="30">
-      <c r="B40" s="52">
+      <c r="B40" s="51">
         <v>38</v>
       </c>
-      <c r="C40" s="53" t="s">
-        <v>218</v>
-      </c>
-      <c r="D40" s="53">
+      <c r="C40" s="52" t="s">
+        <v>217</v>
+      </c>
+      <c r="D40" s="52">
         <v>1</v>
       </c>
-      <c r="E40" s="54">
+      <c r="E40" s="53">
         <v>0.13</v>
       </c>
-      <c r="F40" s="54">
+      <c r="F40" s="53">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="G40" s="53" t="s">
+      <c r="G40" s="52" t="s">
+        <v>218</v>
+      </c>
+      <c r="H40" s="52" t="s">
         <v>219</v>
       </c>
-      <c r="H40" s="53" t="s">
+      <c r="I40" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="52" t="s">
         <v>220</v>
       </c>
-      <c r="I40" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J40" s="53" t="s">
+      <c r="K40" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L40" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M40" s="56" t="s">
         <v>221</v>
-      </c>
-      <c r="K40" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="L40" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="M40" s="57" t="s">
-        <v>222</v>
       </c>
       <c r="N40" s="14"/>
       <c r="O40" s="3"/>
@@ -4621,42 +4666,42 @@
       <c r="AW40" s="3"/>
     </row>
     <row r="41" spans="2:49" ht="30">
-      <c r="B41" s="52">
+      <c r="B41" s="51">
         <v>39</v>
       </c>
-      <c r="C41" s="53" t="s">
-        <v>223</v>
-      </c>
-      <c r="D41" s="53">
+      <c r="C41" s="52" t="s">
+        <v>222</v>
+      </c>
+      <c r="D41" s="52">
         <v>4</v>
       </c>
-      <c r="E41" s="54">
+      <c r="E41" s="53">
         <v>0.13</v>
       </c>
-      <c r="F41" s="54">
+      <c r="F41" s="53">
         <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
-      <c r="G41" s="53" t="s">
+      <c r="G41" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="H41" s="52" t="s">
         <v>224</v>
       </c>
-      <c r="H41" s="53" t="s">
+      <c r="I41" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="52" t="s">
         <v>225</v>
       </c>
-      <c r="I41" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="53" t="s">
+      <c r="K41" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L41" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M41" s="56" t="s">
         <v>226</v>
-      </c>
-      <c r="K41" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="L41" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="M41" s="57" t="s">
-        <v>227</v>
       </c>
       <c r="N41" s="14"/>
       <c r="O41" s="3"/>
@@ -4696,42 +4741,42 @@
       <c r="AW41" s="3"/>
     </row>
     <row r="42" spans="2:49" ht="30">
-      <c r="B42" s="52">
+      <c r="B42" s="51">
         <v>40</v>
       </c>
-      <c r="C42" s="53" t="s">
-        <v>228</v>
-      </c>
-      <c r="D42" s="53">
+      <c r="C42" s="52" t="s">
+        <v>227</v>
+      </c>
+      <c r="D42" s="52">
         <v>2</v>
       </c>
-      <c r="E42" s="54">
+      <c r="E42" s="53">
         <v>0.13</v>
       </c>
-      <c r="F42" s="54">
+      <c r="F42" s="53">
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="G42" s="53" t="s">
+      <c r="G42" s="52" t="s">
+        <v>228</v>
+      </c>
+      <c r="H42" s="52" t="s">
         <v>229</v>
       </c>
-      <c r="H42" s="53" t="s">
+      <c r="I42" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="52" t="s">
         <v>230</v>
       </c>
-      <c r="I42" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="53" t="s">
+      <c r="K42" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L42" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M42" s="56" t="s">
         <v>231</v>
-      </c>
-      <c r="K42" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="L42" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="M42" s="57" t="s">
-        <v>232</v>
       </c>
       <c r="N42" s="14"/>
       <c r="O42" s="3"/>
@@ -4771,42 +4816,42 @@
       <c r="AW42" s="3"/>
     </row>
     <row r="43" spans="2:49" ht="30">
-      <c r="B43" s="52">
+      <c r="B43" s="51">
         <v>41</v>
       </c>
-      <c r="C43" s="53" t="s">
-        <v>233</v>
-      </c>
-      <c r="D43" s="53">
+      <c r="C43" s="52" t="s">
+        <v>232</v>
+      </c>
+      <c r="D43" s="52">
         <v>2</v>
       </c>
-      <c r="E43" s="54">
+      <c r="E43" s="53">
         <v>0.13</v>
       </c>
-      <c r="F43" s="54">
+      <c r="F43" s="53">
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="G43" s="53" t="s">
+      <c r="G43" s="52" t="s">
+        <v>233</v>
+      </c>
+      <c r="H43" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="H43" s="53" t="s">
+      <c r="I43" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" s="52" t="s">
         <v>235</v>
       </c>
-      <c r="I43" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J43" s="53" t="s">
+      <c r="K43" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L43" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M43" s="56" t="s">
         <v>236</v>
-      </c>
-      <c r="K43" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="L43" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="M43" s="57" t="s">
-        <v>237</v>
       </c>
       <c r="N43" s="14"/>
       <c r="O43" s="3"/>
@@ -4846,42 +4891,42 @@
       <c r="AW43" s="3"/>
     </row>
     <row r="44" spans="2:49" ht="30">
-      <c r="B44" s="52">
+      <c r="B44" s="51">
         <v>42</v>
       </c>
-      <c r="C44" s="53" t="s">
-        <v>238</v>
-      </c>
-      <c r="D44" s="53">
+      <c r="C44" s="52" t="s">
+        <v>237</v>
+      </c>
+      <c r="D44" s="52">
         <v>1</v>
       </c>
-      <c r="E44" s="54">
+      <c r="E44" s="53">
         <v>0.13</v>
       </c>
-      <c r="F44" s="54">
+      <c r="F44" s="53">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="G44" s="53" t="s">
+      <c r="G44" s="52" t="s">
+        <v>238</v>
+      </c>
+      <c r="H44" s="52" t="s">
         <v>239</v>
       </c>
-      <c r="H44" s="53" t="s">
+      <c r="I44" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" s="52" t="s">
         <v>240</v>
       </c>
-      <c r="I44" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J44" s="53" t="s">
+      <c r="K44" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L44" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M44" s="56" t="s">
         <v>241</v>
-      </c>
-      <c r="K44" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="L44" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="M44" s="57" t="s">
-        <v>242</v>
       </c>
       <c r="N44" s="14"/>
       <c r="O44" s="3"/>
@@ -4921,42 +4966,42 @@
       <c r="AW44" s="3"/>
     </row>
     <row r="45" spans="2:49" ht="30">
-      <c r="B45" s="52">
+      <c r="B45" s="51">
         <v>43</v>
       </c>
-      <c r="C45" s="53" t="s">
-        <v>244</v>
-      </c>
-      <c r="D45" s="53">
+      <c r="C45" s="52" t="s">
+        <v>243</v>
+      </c>
+      <c r="D45" s="52">
         <v>1</v>
       </c>
-      <c r="E45" s="54">
+      <c r="E45" s="53">
         <v>0.13</v>
       </c>
-      <c r="F45" s="54">
+      <c r="F45" s="53">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="G45" s="53" t="s">
+      <c r="G45" s="52" t="s">
+        <v>244</v>
+      </c>
+      <c r="H45" s="52" t="s">
         <v>245</v>
       </c>
-      <c r="H45" s="53" t="s">
+      <c r="I45" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="52" t="s">
+        <v>242</v>
+      </c>
+      <c r="K45" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="L45" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M45" s="56" t="s">
         <v>246</v>
-      </c>
-      <c r="I45" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J45" s="53" t="s">
-        <v>243</v>
-      </c>
-      <c r="K45" s="53" t="s">
-        <v>181</v>
-      </c>
-      <c r="L45" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="M45" s="57" t="s">
-        <v>247</v>
       </c>
       <c r="N45" s="14"/>
       <c r="O45" s="3"/>
@@ -4996,42 +5041,42 @@
       <c r="AW45" s="3"/>
     </row>
     <row r="46" spans="2:49" ht="30">
-      <c r="B46" s="52">
+      <c r="B46" s="51">
         <v>44</v>
       </c>
-      <c r="C46" s="53" t="s">
-        <v>248</v>
-      </c>
-      <c r="D46" s="53">
+      <c r="C46" s="52" t="s">
+        <v>247</v>
+      </c>
+      <c r="D46" s="52">
         <v>1</v>
       </c>
-      <c r="E46" s="54">
+      <c r="E46" s="53">
         <v>0.13</v>
       </c>
-      <c r="F46" s="54">
+      <c r="F46" s="53">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="G46" s="53" t="s">
+      <c r="G46" s="52" t="s">
+        <v>249</v>
+      </c>
+      <c r="H46" s="52" t="s">
+        <v>248</v>
+      </c>
+      <c r="I46" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="52" t="s">
         <v>250</v>
       </c>
-      <c r="H46" s="53" t="s">
-        <v>249</v>
-      </c>
-      <c r="I46" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="J46" s="53" t="s">
+      <c r="K46" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L46" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M46" s="56" t="s">
         <v>251</v>
-      </c>
-      <c r="K46" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="L46" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="M46" s="57" t="s">
-        <v>252</v>
       </c>
       <c r="N46" s="14"/>
       <c r="O46" s="3"/>
@@ -5075,7 +5120,7 @@
         <v>45</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D47" s="5">
         <v>1</v>
@@ -5088,7 +5133,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>0</v>
@@ -5097,16 +5142,16 @@
         <v>59</v>
       </c>
       <c r="J47" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="K47" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="K47" s="5" t="s">
+      <c r="L47" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M47" s="10" t="s">
         <v>256</v>
-      </c>
-      <c r="L47" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="M47" s="10" t="s">
-        <v>257</v>
       </c>
       <c r="N47" s="14"/>
       <c r="O47" s="3"/>
@@ -5146,42 +5191,42 @@
       <c r="AW47" s="3"/>
     </row>
     <row r="48" spans="2:49" ht="30">
-      <c r="B48" s="59">
+      <c r="B48" s="58">
         <v>46</v>
       </c>
-      <c r="C48" s="60" t="s">
-        <v>258</v>
-      </c>
-      <c r="D48" s="60">
+      <c r="C48" s="59" t="s">
+        <v>257</v>
+      </c>
+      <c r="D48" s="59">
         <v>1</v>
       </c>
-      <c r="E48" s="61">
+      <c r="E48" s="60">
         <v>3.9</v>
       </c>
-      <c r="F48" s="61">
+      <c r="F48" s="60">
         <f t="shared" si="0"/>
         <v>3.9</v>
       </c>
-      <c r="G48" s="60" t="s">
+      <c r="G48" s="59" t="s">
+        <v>262</v>
+      </c>
+      <c r="H48" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="I48" s="59" t="s">
         <v>263</v>
       </c>
-      <c r="H48" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="I48" s="60" t="s">
+      <c r="J48" s="59" t="s">
+        <v>261</v>
+      </c>
+      <c r="K48" s="59" t="s">
         <v>264</v>
       </c>
-      <c r="J48" s="60" t="s">
-        <v>262</v>
-      </c>
-      <c r="K48" s="60" t="s">
+      <c r="L48" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="M48" s="61" t="s">
         <v>265</v>
-      </c>
-      <c r="L48" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="M48" s="62" t="s">
-        <v>266</v>
       </c>
       <c r="N48" s="14"/>
       <c r="O48" s="3"/>
@@ -5221,42 +5266,42 @@
       <c r="AW48" s="3"/>
     </row>
     <row r="49" spans="2:49" ht="30">
-      <c r="B49" s="59">
+      <c r="B49" s="58">
         <v>47</v>
       </c>
-      <c r="C49" s="60" t="s">
-        <v>284</v>
-      </c>
-      <c r="D49" s="60">
+      <c r="C49" s="59" t="s">
+        <v>283</v>
+      </c>
+      <c r="D49" s="59">
         <v>2</v>
       </c>
-      <c r="E49" s="61">
+      <c r="E49" s="60">
         <v>1.56</v>
       </c>
-      <c r="F49" s="61">
+      <c r="F49" s="60">
         <f t="shared" si="0"/>
         <v>3.12</v>
       </c>
-      <c r="G49" s="60" t="s">
+      <c r="G49" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="H49" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="I49" s="59" t="s">
         <v>268</v>
       </c>
-      <c r="H49" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="I49" s="60" t="s">
+      <c r="J49" s="59" t="s">
+        <v>266</v>
+      </c>
+      <c r="K49" s="59" t="s">
         <v>269</v>
       </c>
-      <c r="J49" s="60" t="s">
-        <v>267</v>
-      </c>
-      <c r="K49" s="60" t="s">
+      <c r="L49" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="M49" s="61" t="s">
         <v>270</v>
-      </c>
-      <c r="L49" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="M49" s="62" t="s">
-        <v>271</v>
       </c>
       <c r="N49" s="14"/>
       <c r="O49" s="3"/>
@@ -5296,42 +5341,42 @@
       <c r="AW49" s="3"/>
     </row>
     <row r="50" spans="2:49" ht="30">
-      <c r="B50" s="59">
+      <c r="B50" s="58">
         <v>48</v>
       </c>
-      <c r="C50" s="60" t="s">
-        <v>259</v>
-      </c>
-      <c r="D50" s="60">
+      <c r="C50" s="59" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" s="59">
         <v>1</v>
       </c>
-      <c r="E50" s="61">
+      <c r="E50" s="60">
         <v>61.44</v>
       </c>
-      <c r="F50" s="61">
+      <c r="F50" s="60">
         <f t="shared" si="0"/>
         <v>61.44</v>
       </c>
-      <c r="G50" s="60" t="s">
+      <c r="G50" s="59" t="s">
+        <v>271</v>
+      </c>
+      <c r="H50" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="I50" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="J50" s="59" t="s">
         <v>272</v>
       </c>
-      <c r="H50" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="I50" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="J50" s="60" t="s">
+      <c r="K50" s="59" t="s">
         <v>273</v>
       </c>
-      <c r="K50" s="60" t="s">
+      <c r="L50" s="59" t="s">
+        <v>148</v>
+      </c>
+      <c r="M50" s="61" t="s">
         <v>274</v>
-      </c>
-      <c r="L50" s="60" t="s">
-        <v>149</v>
-      </c>
-      <c r="M50" s="62" t="s">
-        <v>275</v>
       </c>
       <c r="N50" s="14"/>
       <c r="O50" s="3"/>
@@ -5371,42 +5416,42 @@
       <c r="AW50" s="3"/>
     </row>
     <row r="51" spans="2:49" ht="30">
-      <c r="B51" s="59">
+      <c r="B51" s="58">
         <v>49</v>
       </c>
-      <c r="C51" s="60" t="s">
-        <v>260</v>
-      </c>
-      <c r="D51" s="60">
+      <c r="C51" s="59" t="s">
+        <v>259</v>
+      </c>
+      <c r="D51" s="59">
         <v>1</v>
       </c>
-      <c r="E51" s="61">
+      <c r="E51" s="60">
         <v>4.17</v>
       </c>
-      <c r="F51" s="61">
+      <c r="F51" s="60">
         <f t="shared" si="0"/>
         <v>4.17</v>
       </c>
-      <c r="G51" s="60" t="s">
+      <c r="G51" s="59" t="s">
+        <v>276</v>
+      </c>
+      <c r="H51" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="I51" s="59" t="s">
         <v>277</v>
       </c>
-      <c r="H51" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="I51" s="60" t="s">
+      <c r="J51" s="59" t="s">
+        <v>275</v>
+      </c>
+      <c r="K51" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="L51" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="M51" s="61" t="s">
         <v>278</v>
-      </c>
-      <c r="J51" s="60" t="s">
-        <v>276</v>
-      </c>
-      <c r="K51" s="60" t="s">
-        <v>270</v>
-      </c>
-      <c r="L51" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="M51" s="62" t="s">
-        <v>279</v>
       </c>
       <c r="N51" s="14"/>
       <c r="O51" s="3"/>
@@ -5446,42 +5491,42 @@
       <c r="AW51" s="3"/>
     </row>
     <row r="52" spans="2:49" ht="30">
-      <c r="B52" s="59">
+      <c r="B52" s="58">
         <v>50</v>
       </c>
-      <c r="C52" s="60" t="s">
-        <v>261</v>
-      </c>
-      <c r="D52" s="60">
+      <c r="C52" s="59" t="s">
+        <v>260</v>
+      </c>
+      <c r="D52" s="59">
         <v>1</v>
       </c>
-      <c r="E52" s="61">
+      <c r="E52" s="60">
         <v>0.69</v>
       </c>
-      <c r="F52" s="61">
+      <c r="F52" s="60">
         <f t="shared" si="0"/>
         <v>0.69</v>
       </c>
-      <c r="G52" s="60" t="s">
+      <c r="G52" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="H52" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="I52" s="59" t="s">
         <v>280</v>
       </c>
-      <c r="H52" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="I52" s="60" t="s">
+      <c r="J52" s="59" t="s">
         <v>281</v>
       </c>
-      <c r="J52" s="60" t="s">
+      <c r="K52" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="L52" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="M52" s="61" t="s">
         <v>282</v>
-      </c>
-      <c r="K52" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="L52" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="M52" s="62" t="s">
-        <v>283</v>
       </c>
       <c r="N52" s="14"/>
       <c r="O52" s="3"/>
@@ -5525,7 +5570,7 @@
         <v>51</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D53" s="5">
         <v>1</v>
@@ -5538,25 +5583,25 @@
         <v>0.92</v>
       </c>
       <c r="G53" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="H53" s="5" t="s">
         <v>287</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>288</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>59</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K53" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M53" s="10" t="s">
         <v>289</v>
-      </c>
-      <c r="L53" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="M53" s="10" t="s">
-        <v>290</v>
       </c>
       <c r="N53" s="14"/>
       <c r="O53" s="3"/>
@@ -5600,7 +5645,7 @@
         <v>52</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D54" s="5">
         <v>1</v>
@@ -5613,22 +5658,22 @@
         <v>5.71</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J54" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K54" s="5" t="s">
         <v>2</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M54" s="10" t="s">
         <v>1</v>
@@ -5675,41 +5720,41 @@
         <v>53</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D55" s="16">
         <v>1</v>
       </c>
-      <c r="E55" s="20">
+      <c r="E55" s="66">
         <v>14.95</v>
       </c>
-      <c r="F55" s="20">
+      <c r="F55" s="66">
         <f t="shared" si="0"/>
         <v>14.95</v>
       </c>
       <c r="G55" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="H55" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="H55" s="16" t="s">
+      <c r="I55" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="I55" s="16" t="s">
+      <c r="J55" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="J55" s="17" t="s">
+      <c r="K55" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="K55" s="16" t="s">
+      <c r="L55" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="M55" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="L55" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="M55" s="18" t="s">
-        <v>300</v>
-      </c>
       <c r="N55" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
@@ -5747,12 +5792,17 @@
       <c r="AV55" s="3"/>
       <c r="AW55" s="3"/>
     </row>
-    <row r="56" spans="2:49">
+    <row r="56" spans="2:49" ht="13.5" thickBot="1">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
+      <c r="E56" s="67" t="s">
+        <v>300</v>
+      </c>
+      <c r="F56" s="68">
+        <f>SUM(F3:F55)</f>
+        <v>125.44</v>
+      </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>

</xml_diff>